<commit_message>
some change by zq
</commit_message>
<xml_diff>
--- a/src/excelhandler/student.xlsx
+++ b/src/excelhandler/student.xlsx
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>